<commit_message>
kerman link excel modified
</commit_message>
<xml_diff>
--- a/kerman/link_kerman.xlsx
+++ b/kerman/link_kerman.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Desktop\kerman\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Desktop\NetPlanner\kerman\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="32">
   <si>
     <t>K4</t>
   </si>
@@ -607,7 +607,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -794,6 +794,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="201">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1136,7 +1147,7 @@
     </xf>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="29" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1157,6 +1168,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="27" borderId="16" xfId="200" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="28" borderId="16" xfId="200" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1639,10 +1656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1741,7 +1758,7 @@
         <v>1.4E-3</v>
       </c>
       <c r="I3" s="6">
-        <f t="shared" ref="I3:I33" si="0">POWER(4.8434, -27)</f>
+        <f t="shared" ref="I3:I34" si="0">POWER(4.8434, -27)</f>
         <v>3.169136089868813E-19</v>
       </c>
     </row>
@@ -2641,6 +2658,36 @@
         <v>1.4E-3</v>
       </c>
       <c r="I33" s="6">
+        <f t="shared" si="0"/>
+        <v>3.169136089868813E-19</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="8">
+        <v>33</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" s="6">
+        <v>84</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F34" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="G34" s="6">
+        <v>0</v>
+      </c>
+      <c r="H34" s="7">
+        <v>1.4E-3</v>
+      </c>
+      <c r="I34" s="6">
         <f t="shared" si="0"/>
         <v>3.169136089868813E-19</v>
       </c>

</xml_diff>